<commit_message>
Add data generation scripts for Monte Carlo simulations
- Created plot_data_generator__csv__v1.py to generate CSV data for 50 scenarios with specified KPIs and years.
- Created plot_data_generator__json.py to generate JSON data for the same scenarios, including metadata.
- Introduced plot_data_generator__csv__v2.py with command-line argument support for customizable scenarios and years.
</commit_message>
<xml_diff>
--- a/montecarlo/montecarlo_input_template5.xlsx
+++ b/montecarlo/montecarlo_input_template5.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://intesasanpaolo-my.sharepoint.com/personal/stefano_spinucci_intesasanpaolo_com/Documents/mci/zzz python dashboard/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\e3\@gitwk\PUBLIC\financial-modeling\montecarlo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="291" documentId="11_F7D251F714787E0FE779D97DBFD9464199442EE7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{62D7904B-4CAA-4E21-B299-29586A3678D0}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBE014E8-1A35-4862-A4AD-653CB32F20DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13866" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="instructions" sheetId="6" r:id="rId1"/>
@@ -38,6 +38,7 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>GPT</author>
+    <author>Stefano Spinucci</author>
   </authors>
   <commentList>
     <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
@@ -51,6 +52,35 @@
             <scheme val="minor"/>
           </rPr>
           <t>For discrete variables only. Each (variable,month) must have rows covering all outcomes.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="1" shapeId="0" xr:uid="{798AA851-77BA-414B-981D-F21E72259EE4}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>field used by Montecarlo data extraction to select a value from generated data;
+not used for data generation</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G1" authorId="1" shapeId="0" xr:uid="{B49DA41F-9ED1-44A7-B54E-E97CB4967245}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>field unsed by Montecarlo data generation and extraction</t>
         </r>
       </text>
     </comment>
@@ -251,7 +281,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -264,6 +294,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -291,7 +328,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -611,109 +648,109 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>46</v>
       </c>
@@ -728,21 +765,21 @@
   <dimension ref="A1:G52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.41015625" customWidth="1"/>
-    <col min="2" max="2" width="16.41015625" customWidth="1"/>
-    <col min="3" max="3" width="14.87890625" customWidth="1"/>
-    <col min="4" max="4" width="20.3515625" customWidth="1"/>
-    <col min="5" max="5" width="16.52734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.3515625" customWidth="1"/>
+    <col min="1" max="1" width="17.44140625" customWidth="1"/>
+    <col min="2" max="2" width="16.44140625" customWidth="1"/>
+    <col min="3" max="3" width="14.88671875" customWidth="1"/>
+    <col min="4" max="4" width="20.33203125" customWidth="1"/>
+    <col min="5" max="5" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.33203125" customWidth="1"/>
     <col min="7" max="7" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -765,7 +802,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -785,7 +822,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -802,7 +839,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -822,7 +859,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -836,7 +873,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -853,7 +890,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -867,7 +904,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -884,7 +921,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -898,7 +935,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -915,7 +952,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -929,7 +966,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -946,7 +983,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -960,7 +997,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -977,7 +1014,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -991,7 +1028,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>21</v>
       </c>
@@ -1008,7 +1045,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>21</v>
       </c>
@@ -1022,7 +1059,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -1039,7 +1076,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>21</v>
       </c>
@@ -1053,7 +1090,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -1070,7 +1107,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -1084,7 +1121,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -1101,7 +1138,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -1115,7 +1152,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>21</v>
       </c>
@@ -1132,7 +1169,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>21</v>
       </c>
@@ -1146,7 +1183,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>21</v>
       </c>
@@ -1163,7 +1200,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>21</v>
       </c>
@@ -1177,7 +1214,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>21</v>
       </c>
@@ -1194,7 +1231,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>21</v>
       </c>
@@ -1208,7 +1245,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>21</v>
       </c>
@@ -1225,7 +1262,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="31" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>21</v>
       </c>
@@ -1239,7 +1276,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="32" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>21</v>
       </c>
@@ -1256,7 +1293,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="33" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>21</v>
       </c>
@@ -1270,7 +1307,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="34" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>21</v>
       </c>
@@ -1287,7 +1324,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="35" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>21</v>
       </c>
@@ -1301,7 +1338,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="36" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>21</v>
       </c>
@@ -1318,7 +1355,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="37" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>21</v>
       </c>
@@ -1332,7 +1369,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="38" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>21</v>
       </c>
@@ -1349,7 +1386,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="39" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>21</v>
       </c>
@@ -1363,7 +1400,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="40" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>21</v>
       </c>
@@ -1380,7 +1417,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="41" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>21</v>
       </c>
@@ -1394,7 +1431,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="42" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>21</v>
       </c>
@@ -1411,7 +1448,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="43" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>21</v>
       </c>
@@ -1425,7 +1462,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="44" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>21</v>
       </c>
@@ -1442,7 +1479,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="45" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>21</v>
       </c>
@@ -1456,7 +1493,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="46" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>21</v>
       </c>
@@ -1473,7 +1510,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="47" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>21</v>
       </c>
@@ -1487,7 +1524,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="48" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>21</v>
       </c>
@@ -1504,7 +1541,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="49" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>21</v>
       </c>
@@ -1518,7 +1555,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B50" t="s">
         <v>3</v>
       </c>
@@ -1532,7 +1569,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B51" t="s">
         <v>3</v>
       </c>
@@ -1546,7 +1583,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B52" t="s">
         <v>3</v>
       </c>
@@ -1578,13 +1615,13 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="12" customWidth="1"/>
     <col min="3" max="3" width="40" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -1595,7 +1632,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -1606,7 +1643,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -1617,7 +1654,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>14</v>
       </c>

</xml_diff>